<commit_message>
push with some histogram changes
</commit_message>
<xml_diff>
--- a/WeatherData.xlsx
+++ b/WeatherData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahd\Documents\SimulationRocketPy\RocketPy-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F296EF12-89BB-48BD-9913-E83656AF320B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9ED1A18-CBC1-4C22-AEBA-A12A1A6345D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1A62284C-9F49-4E28-BF1D-693DB80445E5}"/>
+    <workbookView xWindow="5760" yWindow="12" windowWidth="17280" windowHeight="8880" xr2:uid="{1A62284C-9F49-4E28-BF1D-693DB80445E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>https://weather.uwyo.edu/cgi-bin/sounding?region=naconf&amp;TYPE=TEXT%3ALIST&amp;YEAR=2024&amp;MONTH=04&amp;FROM=0200&amp;TO=2412&amp;STNM=72249</t>
-  </si>
-  <si>
-    <t>https://rucsoundings.noaa.gov/get_soundings.cgi?data_source=GFS&amp;latest=latest&amp;start_year=2024&amp;start_month_name=Sep&amp;start_mday=11&amp;start_hour=1&amp;start_min=0&amp;n_hrs=24&amp;fcst_len=shortest&amp;airport=&amp;start=latest</t>
   </si>
 </sst>
 </file>
@@ -404,11 +401,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143EB736-08E8-4914-B337-69775041A995}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -417,33 +412,18 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{AF8D2003-08A2-4217-BEAF-75FEBE5F6615}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{4193A3BD-9933-480F-AE77-8587BEFEA1D5}"/>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{4193A3BD-9933-480F-AE77-8587BEFEA1D5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A47D3F95C322F46B81E26B010C8A6F1" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b721691e22b01c92effc85e5907ff3e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b87b9a2c-4f2f-4e8d-b7ed-efd8c43dbad6" xmlns:ns4="13bd0b69-687f-4121-b60e-319cf29d7719" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dfd4db8eb86c76d32938a1b9d1e1eda4" ns3:_="" ns4:_="">
     <xsd:import namespace="b87b9a2c-4f2f-4e8d-b7ed-efd8c43dbad6"/>
@@ -626,6 +606,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -635,14 +624,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF8B8B5A-B969-4CE4-B367-43CE86BA4FFF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9854CF6-6509-4BD5-8909-1C888FF32DF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -661,6 +642,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF8B8B5A-B969-4CE4-B367-43CE86BA4FFF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10ADC3BF-90E4-4507-B601-CE608BDBF35E}">
   <ds:schemaRefs>

</xml_diff>